<commit_message>
update create form for staff
</commit_message>
<xml_diff>
--- a/database/template/init_form.xlsx
+++ b/database/template/init_form.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="385">
   <si>
     <t>item_k</t>
   </si>
@@ -163,10 +163,6 @@
     <t>1: 1-phase
 2: 3-phase
 3: None</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ប្រភេទនៃខ្សែពីម៉ែត្រទៅស្ថានីយ៍
-</t>
   </si>
   <si>
     <t>Cable Type from Meter to Station</t>
@@ -213,10 +209,6 @@
 7: None</t>
   </si>
   <si>
-    <t xml:space="preserve">ស្ថានីយ៍មាន CB Mមុនចូលស្ថានីយ៍ទេ?
-</t>
-  </si>
-  <si>
     <t>Does the station have CB M before entering the station?</t>
   </si>
   <si>
@@ -266,10 +258,6 @@
     <t>1: Yes
 2: No
 3: None</t>
-  </si>
-  <si>
-    <t xml:space="preserve">តើស្ថានីយ៍ភលើងខ្សោយដែលអាចភ្ជាប់ 3P បានទេ?
-</t>
   </si>
   <si>
     <t>Can the low voltage station connect to 3P?</t>
@@ -551,10 +539,6 @@
 1: Tủ không có vị trí lắp
 2: Trạm có kế hoạch hủy/ di dời.
 3. Khác</t>
-  </si>
-  <si>
-    <t xml:space="preserve">តើស្ថានីយអាចដំឡើងទូប្រភេទខាងក្រៅថែមបានទេ?
-</t>
   </si>
   <si>
     <t>Can the Station Install Additional Outdoor Units?</t>
@@ -601,9 +585,6 @@
 3: trạm có KH hủy/di dời
 4: trạm dân kiện/ Chủ nhà không cho lắp đặt bổ sung
 5: khác</t>
-  </si>
-  <si>
-    <t>ម៉ូឌែលទូរទតុងអាគុយខាងក្រៅ</t>
   </si>
   <si>
     <t>Outdoor Battery Rack Model</t>
@@ -661,10 +642,6 @@
     <t>can_install_additional_outdoor_battery_units</t>
   </si>
   <si>
-    <t xml:space="preserve">មូលហេតុដែលមិនអាចដំឡើងទូដាក់ថ្មខាងក្រៅបាន
-</t>
-  </si>
-  <si>
     <t>Reason for Not Being Able to Install Outdoor Battery Units</t>
   </si>
   <si>
@@ -767,11 +744,6 @@
 3: 25mm2
 4: 35mm2
 5: None</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ប្រភេទផ្ទុះម៉ាស៊ីនដែលកំពុងប្រើប្រាស់៖
-0: គ្មាន
-</t>
   </si>
   <si>
     <t>Generator Type in Use</t>
@@ -2169,6 +2141,36 @@
     <t>1: 1
 2: 2
 3: 3</t>
+  </si>
+  <si>
+    <t>ចំនួន​ racks 19"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">មូលហេតុដែលមិនដំឡើងទូដាក់អាគុយខាងក្រៅបាន
+</t>
+  </si>
+  <si>
+    <t>ម៉ូឌែលទូរដាក់អាគុយខាងក្រៅ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ប្រភេទផ្ទះម៉ាស៊ីនដែលកំពុងប្រើប្រាស់៖ ​0: គ្មាន
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">តើស្ថានីយ៏ភ្លើងខ្សោយដែលអាចភ្ជាប់ឡើង​ 3​P បានទេ?
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ស្ថានីយ៏មាន MCB មុនចូលស្ថានីយ៏ទេ?
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">តើស្ថានីយ៍អាចដំឡើងឧបករណ៍ខាងក្រៅបន្ថែមបានទេ?
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ប្រភេទខ្សែពីម៉ែត្រទ័រទៅស្ថានីយ៏
+</t>
   </si>
 </sst>
 </file>
@@ -2601,13 +2603,13 @@
   <dimension ref="A1:H75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="37.5546875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
     <col min="3" max="3" width="29.33203125" customWidth="1"/>
     <col min="4" max="4" width="14.44140625" customWidth="1"/>
     <col min="5" max="5" width="21.109375" customWidth="1"/>
@@ -2788,10 +2790,10 @@
         <v>39</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="93.6">
@@ -2812,95 +2814,95 @@
         <v>44</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="109.2">
       <c r="A11" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="G11" s="2" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="156">
       <c r="A12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="D12" s="5">
         <v>1</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="G12" s="2" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="78">
       <c r="A13" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="109.2">
       <c r="A14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="D14" s="5">
         <v>1</v>
@@ -2912,225 +2914,225 @@
         <v>39</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="93.6">
       <c r="A15" s="2" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="140.4">
       <c r="A16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="156">
       <c r="A17" s="2" t="s">
-        <v>70</v>
+        <v>381</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="124.8">
       <c r="A18" s="2" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="78">
       <c r="A19" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D19" s="5">
         <v>1</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="46.8">
       <c r="A20" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="78">
       <c r="A21" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D21" s="5">
         <v>1</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="46.8">
       <c r="A22" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="46.8">
       <c r="A23" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="2" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="G23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H23" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="62.4">
       <c r="A24" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D24" s="5">
         <v>1</v>
@@ -3138,89 +3140,89 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="109.2">
       <c r="A25" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="140.4">
       <c r="A26" s="2" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="156">
       <c r="A27" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H27" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="62.4">
       <c r="A28" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D28" s="5">
         <v>1</v>
@@ -3228,89 +3230,89 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="109.2">
       <c r="A29" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="140.4">
       <c r="A30" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="156">
       <c r="A31" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="62.4">
       <c r="A32" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D32" s="5">
         <v>1</v>
@@ -3318,733 +3320,733 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="109.2">
       <c r="A33" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="140.4">
       <c r="A34" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="156">
       <c r="A35" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="234">
       <c r="A36" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D36" s="5">
         <v>1</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="140.4">
       <c r="A37" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="171.6">
       <c r="A38" s="2" t="s">
-        <v>149</v>
+        <v>383</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D38" s="5">
         <v>1</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="280.8">
       <c r="A39" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="109.2">
       <c r="A40" s="6" t="s">
-        <v>159</v>
+        <v>379</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D40" s="5">
         <v>1</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="156">
       <c r="A41" s="6" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D41" s="5">
         <v>1</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="171.6">
       <c r="A42" s="6" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="280.8">
       <c r="A43" s="6" t="s">
-        <v>172</v>
+        <v>378</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="6" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="78">
       <c r="A44" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D44" s="5">
         <v>1</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="109.2">
       <c r="A45" s="2" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="2" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="62.4">
       <c r="A46" s="2" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="140.4">
       <c r="A47" s="2" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="187.2">
       <c r="A48" s="2" t="s">
-        <v>196</v>
+        <v>380</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="D48" s="5">
         <v>1</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="109.2">
       <c r="A49" s="2" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="2" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="109.2">
       <c r="A50" s="2" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="2" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="187.2">
       <c r="A51" s="2" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="2" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="124.8">
       <c r="A52" s="2" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="2" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="78">
       <c r="A53" s="2" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="78">
       <c r="A54" s="2" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="93.6">
       <c r="A55" s="2" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="62.4">
       <c r="A56" s="2" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="62.4">
       <c r="A57" s="2" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="2" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="62.4">
       <c r="A58" s="2" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="2" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="46.8">
       <c r="A59" s="2" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="62.4">
       <c r="A60" s="2" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="2" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="62.4">
       <c r="A61" s="2" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="46.8">
       <c r="A62" s="2" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="2" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="15.6">
       <c r="A63" s="2" t="s">
-        <v>276</v>
+        <v>377</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="D63" s="5">
         <v>1</v>
@@ -4052,137 +4054,137 @@
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="78">
       <c r="A64" s="2" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="D64" s="5">
         <v>1</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="46.8">
       <c r="A65" s="2" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="202.8">
       <c r="A66" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="D66" s="5">
         <v>1</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="46.8">
       <c r="A67" s="2" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
       <c r="G67" s="2" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="156">
       <c r="A68" s="2" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="2" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="46.8">
       <c r="A69" s="2" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="D69" s="5">
         <v>1</v>
@@ -4190,152 +4192,152 @@
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="124.8">
       <c r="A70" s="2" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="D70" s="5">
         <v>1</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="46.8">
       <c r="A71" s="2" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="187.2">
       <c r="A72" s="2" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="2" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="78">
       <c r="A73" s="2" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="109.2">
       <c r="A74" s="2" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="249.6">
       <c r="A75" s="2" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="2" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update user in admin and set select option in create site
</commit_message>
<xml_diff>
--- a/database/template/init_form.xlsx
+++ b/database/template/init_form.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="387">
   <si>
     <t>item_k</t>
   </si>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t>room_type_in_station</t>
-  </si>
-  <si>
-    <t>Loại nhà trạm</t>
   </si>
   <si>
     <t xml:space="preserve">CB EDC
@@ -2171,6 +2168,36 @@
   <si>
     <t xml:space="preserve">ប្រភេទខ្សែពីម៉ែត្រទ័រទៅស្ថានីយ៏
 </t>
+  </si>
+  <si>
+    <t>1: Outdoor (មានទូសំភារះ + មានទូអាគុយ)
+2: Outdoor (មានតែទូសំភារះ ឬ ទូដេសេ​តែមួយ)
+3: បន្ទប់ថ្ម
+4: បន្ទប់កុងតែន័រ
+5: ក្នុងអគា
+6: RRU
+7: AAU
+8: បន្ទប់សំណាញ់​ (បិតស័ង្កសីជុំវិញ)</t>
+  </si>
+  <si>
+    <t>1: Outdoor (with equipment cabinet + battery cabinet)
+2: Outdoor (only equipment cabinet or single cabinet)
+3: Battery room
+4: Container room
+5: Indoor
+6: RRU
+7: AAU
+8: Glass room (covered with zinc around)</t>
+  </si>
+  <si>
+    <t>1: Outdoor (មានទូសំភារះ + មានទូអាគុយ)
+2: Outdoor (មានតែទូសំភារះ ឬ ទូដេសេ​តែមួយ)
+3: បន្ទប់ថ្ម (xây)
+4: បន្ទប់កុងតែន័រ (Conteno)
+5: ក្នុងអគា (trong nhà)
+6: RRU
+7: AAU
+8: បន្ទប់សំណាញ់​ (បិតស័ង្កសីជុំវិញ) (quây tôn)</t>
   </si>
 </sst>
 </file>
@@ -2602,8 +2629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2612,8 +2639,8 @@
     <col min="2" max="2" width="23.6640625" customWidth="1"/>
     <col min="3" max="3" width="29.33203125" customWidth="1"/>
     <col min="4" max="4" width="14.44140625" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="39.6640625" customWidth="1"/>
+    <col min="6" max="6" width="49.77734375" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
     <col min="8" max="8" width="32.5546875" customWidth="1"/>
   </cols>
@@ -2752,7 +2779,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="17.399999999999999">
+    <row r="8" spans="1:8" ht="202.8">
       <c r="A8" s="2" t="s">
         <v>32</v>
       </c>
@@ -2763,376 +2790,382 @@
         <v>34</v>
       </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>384</v>
+      </c>
       <c r="H8" s="5" t="s">
-        <v>35</v>
+        <v>386</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="109.2">
       <c r="A9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="D9" s="5">
         <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>331</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="93.6">
       <c r="A10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="G10" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>333</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="109.2">
       <c r="A11" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="G11" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>335</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="156">
       <c r="A12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="D12" s="5">
         <v>1</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="G12" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>337</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="78">
       <c r="A13" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="109.2">
       <c r="A14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="D14" s="5">
         <v>1</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G14" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="H14" s="5" t="s">
         <v>339</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="93.6">
       <c r="A15" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>341</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="140.4">
       <c r="A16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G16" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>343</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="156">
       <c r="A17" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G17" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>345</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="124.8">
       <c r="A18" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>347</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="78">
       <c r="A19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="D19" s="5">
         <v>1</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G19" s="2" t="s">
+      <c r="H19" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="46.8">
       <c r="A20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>80</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H20" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="78">
       <c r="A21" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="D21" s="5">
         <v>1</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G21" s="2" t="s">
+      <c r="H21" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="46.8">
       <c r="A22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H22" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="46.8">
       <c r="A23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="62.4">
       <c r="A24" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="D24" s="5">
         <v>1</v>
@@ -3140,89 +3173,89 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H24" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="109.2">
       <c r="A25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G25" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H25" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="140.4">
       <c r="A26" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="H26" s="5" t="s">
         <v>350</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="156">
       <c r="A27" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="H27" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="62.4">
       <c r="A28" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>114</v>
       </c>
       <c r="D28" s="5">
         <v>1</v>
@@ -3230,89 +3263,89 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H28" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="109.2">
       <c r="A29" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G29" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H29" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="140.4">
       <c r="A30" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>120</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="156">
       <c r="A31" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="H31" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="62.4">
       <c r="A32" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="D32" s="5">
         <v>1</v>
@@ -3320,733 +3353,733 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H32" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="109.2">
       <c r="A33" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G33" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H33" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="140.4">
       <c r="A34" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="156">
       <c r="A35" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>137</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="H35" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="234">
       <c r="A36" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>140</v>
       </c>
       <c r="D36" s="5">
         <v>1</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G36" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="H36" s="5" t="s">
         <v>353</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="140.4">
       <c r="A37" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>143</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H37" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="171.6">
       <c r="A38" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>147</v>
       </c>
       <c r="D38" s="5">
         <v>1</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="H38" s="5" t="s">
         <v>355</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="280.8">
       <c r="A39" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="G39" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="H39" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="109.2">
       <c r="A40" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>156</v>
       </c>
       <c r="D40" s="5">
         <v>1</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G40" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="H40" s="7" t="s">
         <v>157</v>
-      </c>
-      <c r="H40" s="7" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="156">
       <c r="A41" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>161</v>
       </c>
       <c r="D41" s="5">
         <v>1</v>
       </c>
       <c r="E41" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="H41" s="7" t="s">
         <v>162</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="H41" s="7" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="171.6">
       <c r="A42" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>165</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>166</v>
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G42" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="H42" s="7" t="s">
         <v>357</v>
-      </c>
-      <c r="H42" s="7" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="280.8">
       <c r="A43" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>168</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="F43" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="G43" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="G43" s="6" t="s">
+      <c r="H43" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="H43" s="7" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="78">
       <c r="A44" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>175</v>
       </c>
       <c r="D44" s="5">
         <v>1</v>
       </c>
       <c r="E44" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="G44" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="H44" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="H44" s="5" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="109.2">
       <c r="A45" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="C45" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G45" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="H45" s="5" t="s">
         <v>359</v>
-      </c>
-      <c r="H45" s="5" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="62.4">
       <c r="A46" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>184</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>185</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="H46" s="5" t="s">
         <v>361</v>
-      </c>
-      <c r="H46" s="5" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="140.4">
       <c r="A47" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>187</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>188</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G47" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="H47" s="5" t="s">
         <v>363</v>
-      </c>
-      <c r="H47" s="5" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="187.2">
       <c r="A48" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>191</v>
       </c>
       <c r="D48" s="5">
         <v>1</v>
       </c>
       <c r="E48" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="G48" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="H48" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="H48" s="5" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="109.2">
       <c r="A49" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="C49" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>198</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G49" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="H49" s="5" t="s">
         <v>365</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="109.2">
       <c r="A50" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="C50" s="3" t="s">
         <v>201</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>202</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="F50" s="2" t="s">
-        <v>204</v>
-      </c>
       <c r="G50" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="H50" s="5" t="s">
         <v>367</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="187.2">
       <c r="A51" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="C51" s="3" t="s">
         <v>206</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>207</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="G51" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="G51" s="2" t="s">
+      <c r="H51" s="5" t="s">
         <v>210</v>
-      </c>
-      <c r="H51" s="5" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="124.8">
       <c r="A52" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="C52" s="3" t="s">
         <v>213</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>214</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="G52" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="G52" s="2" t="s">
+      <c r="H52" s="5" t="s">
         <v>217</v>
-      </c>
-      <c r="H52" s="5" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="78">
       <c r="A53" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="C53" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>221</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="78">
       <c r="A54" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B54" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="C54" s="8" t="s">
         <v>224</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>225</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G54" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="H54" s="5" t="s">
         <v>226</v>
-      </c>
-      <c r="H54" s="5" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="93.6">
       <c r="A55" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B55" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="C55" s="8" t="s">
         <v>229</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>230</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G55" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="H55" s="5" t="s">
         <v>231</v>
-      </c>
-      <c r="H55" s="5" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="62.4">
       <c r="A56" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B56" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="C56" s="8" t="s">
         <v>234</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>235</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G56" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="H56" s="5" t="s">
         <v>236</v>
-      </c>
-      <c r="H56" s="5" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="62.4">
       <c r="A57" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B57" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="C57" s="8" t="s">
         <v>239</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>240</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="G57" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="F57" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="G57" s="2" t="s">
+      <c r="H57" s="5" t="s">
         <v>242</v>
-      </c>
-      <c r="H57" s="5" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="62.4">
       <c r="A58" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B58" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="C58" s="8" t="s">
         <v>245</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>246</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G58" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="F58" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="G58" s="2" t="s">
+      <c r="H58" s="5" t="s">
         <v>248</v>
-      </c>
-      <c r="H58" s="5" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="46.8">
       <c r="A59" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B59" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="C59" s="8" t="s">
         <v>251</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>252</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G59" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="H59" s="5" t="s">
         <v>253</v>
-      </c>
-      <c r="H59" s="5" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="62.4">
       <c r="A60" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B60" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="B60" s="8" t="s">
+      <c r="C60" s="8" t="s">
         <v>256</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>257</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G60" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="H60" s="5" t="s">
         <v>258</v>
-      </c>
-      <c r="H60" s="5" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="62.4">
       <c r="A61" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B61" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="B61" s="8" t="s">
+      <c r="C61" s="8" t="s">
         <v>261</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>262</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="46.8">
       <c r="A62" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B62" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="B62" s="8" t="s">
+      <c r="C62" s="8" t="s">
         <v>265</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>266</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G62" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="H62" s="5" t="s">
         <v>267</v>
-      </c>
-      <c r="H62" s="5" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="15.6">
       <c r="A63" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B63" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="C63" s="8" t="s">
         <v>270</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>271</v>
       </c>
       <c r="D63" s="5">
         <v>1</v>
@@ -4054,137 +4087,137 @@
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="78">
       <c r="A64" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B64" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="C64" s="8" t="s">
         <v>274</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>275</v>
       </c>
       <c r="D64" s="5">
         <v>1</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G64" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="H64" s="5" t="s">
         <v>276</v>
-      </c>
-      <c r="H64" s="5" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="46.8">
       <c r="A65" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B65" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="C65" s="8" t="s">
         <v>279</v>
-      </c>
-      <c r="C65" s="8" t="s">
-        <v>280</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="202.8">
       <c r="A66" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B66" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="B66" s="8" t="s">
+      <c r="C66" s="8" t="s">
         <v>283</v>
-      </c>
-      <c r="C66" s="8" t="s">
-        <v>284</v>
       </c>
       <c r="D66" s="5">
         <v>1</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G66" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="H66" s="5" t="s">
         <v>369</v>
-      </c>
-      <c r="H66" s="5" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="46.8">
       <c r="A67" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B67" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="B67" s="8" t="s">
+      <c r="C67" s="8" t="s">
         <v>286</v>
-      </c>
-      <c r="C67" s="8" t="s">
-        <v>287</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
       <c r="G67" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="156">
       <c r="A68" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B68" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="B68" s="8" t="s">
+      <c r="C68" s="8" t="s">
         <v>290</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>291</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="F68" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="F68" s="2" t="s">
+      <c r="G68" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="G68" s="2" t="s">
+      <c r="H68" s="5" t="s">
         <v>294</v>
-      </c>
-      <c r="H68" s="5" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="46.8">
       <c r="A69" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B69" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="B69" s="8" t="s">
+      <c r="C69" s="8" t="s">
         <v>297</v>
-      </c>
-      <c r="C69" s="8" t="s">
-        <v>298</v>
       </c>
       <c r="D69" s="5">
         <v>1</v>
@@ -4192,152 +4225,152 @@
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="124.8">
       <c r="A70" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B70" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="B70" s="8" t="s">
+      <c r="C70" s="8" t="s">
         <v>301</v>
-      </c>
-      <c r="C70" s="8" t="s">
-        <v>302</v>
       </c>
       <c r="D70" s="5">
         <v>1</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G70" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="H70" s="5" t="s">
         <v>371</v>
-      </c>
-      <c r="H70" s="5" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="46.8">
       <c r="A71" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B71" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="B71" s="8" t="s">
+      <c r="C71" s="8" t="s">
         <v>304</v>
-      </c>
-      <c r="C71" s="8" t="s">
-        <v>305</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="187.2">
       <c r="A72" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B72" s="8" t="s">
         <v>307</v>
       </c>
-      <c r="B72" s="8" t="s">
+      <c r="C72" s="8" t="s">
         <v>308</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>309</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="F72" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="F72" s="2" t="s">
+      <c r="G72" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="G72" s="2" t="s">
+      <c r="H72" s="5" t="s">
         <v>312</v>
-      </c>
-      <c r="H72" s="5" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="78">
       <c r="A73" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B73" s="8" t="s">
         <v>314</v>
       </c>
-      <c r="B73" s="8" t="s">
+      <c r="C73" s="8" t="s">
         <v>315</v>
-      </c>
-      <c r="C73" s="8" t="s">
-        <v>316</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G73" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="H73" s="5" t="s">
         <v>317</v>
-      </c>
-      <c r="H73" s="5" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="109.2">
       <c r="A74" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B74" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="B74" s="8" t="s">
+      <c r="C74" s="8" t="s">
         <v>320</v>
-      </c>
-      <c r="C74" s="8" t="s">
-        <v>321</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G74" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="H74" s="5" t="s">
         <v>322</v>
-      </c>
-      <c r="H74" s="5" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="249.6">
       <c r="A75" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B75" s="8" t="s">
         <v>324</v>
       </c>
-      <c r="B75" s="8" t="s">
+      <c r="C75" s="8" t="s">
         <v>325</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>326</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="F75" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="G75" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="G75" s="2" t="s">
+      <c r="H75" s="5" t="s">
         <v>329</v>
-      </c>
-      <c r="H75" s="5" t="s">
-        <v>330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>